<commit_message>
power results for k=2 adjusted such that d=0.084, as when k=3
</commit_message>
<xml_diff>
--- a/Outputs/power quantification/Power simulations .xlsx
+++ b/Outputs/power quantification/Power simulations .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\Outputs\power quantification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7135B740-86FB-47BF-83A0-FAA476770E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E460F5-DEFC-42D3-ADDA-DC33B9810170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10740" yWindow="300" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>n</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>new n (based on d=0.084)</t>
   </si>
 </sst>
 </file>
@@ -431,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E504A511-A259-4903-8689-62EE7A3DA240}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -455,8 +458,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -472,8 +478,11 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,8 +498,11 @@
       <c r="E3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -506,8 +518,11 @@
       <c r="E4">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -523,8 +538,11 @@
       <c r="E5">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -540,8 +558,11 @@
       <c r="E6">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -557,8 +578,11 @@
       <c r="E7">
         <v>167</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -574,8 +598,11 @@
       <c r="E8">
         <v>257</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -591,8 +618,11 @@
       <c r="E9">
         <v>391</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -608,8 +638,11 @@
       <c r="E10">
         <v>586</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -625,8 +658,11 @@
       <c r="E11">
         <v>976</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -642,8 +678,11 @@
       <c r="E12">
         <v>1952</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -660,7 +699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -677,7 +716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -694,7 +733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>

</xml_diff>